<commit_message>
python to get excel
</commit_message>
<xml_diff>
--- a/AppSpecification.xlsx
+++ b/AppSpecification.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="132" yWindow="600" windowWidth="22716" windowHeight="10788"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -34,36 +37,37 @@
     <t>Remaining</t>
   </si>
   <si>
-    <t>annual</t>
-  </si>
-  <si>
     <t>monthly</t>
   </si>
   <si>
     <t>quarterly</t>
+  </si>
+  <si>
+    <t>annually</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -71,7 +75,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,56 +85,45 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -320,24 +313,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="4" width="16.86"/>
-    <col customWidth="1" min="7" max="7" width="3.0"/>
+    <col min="3" max="4" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -361,52 +359,51 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>10000.0</v>
+        <v>10000</v>
       </c>
       <c r="B2" s="3">
-        <v>43831.0</v>
+        <v>43831</v>
       </c>
       <c r="C2" s="3">
-        <v>43876.0</v>
+        <v>43876</v>
       </c>
       <c r="D2" s="1">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="4">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="7">
         <f>A2-D2+87</f>
         <v>9087</v>
       </c>
-      <c r="N2" s="8"/>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A5" si="1">H2</f>
+        <f t="shared" ref="A3:A5" si="0">H2</f>
         <v>9087</v>
       </c>
-      <c r="B3" s="9">
-        <f t="shared" ref="B3:B5" si="2">C2</f>
+      <c r="B3" s="8">
+        <f t="shared" ref="B3:B5" si="1">C2</f>
         <v>43876</v>
       </c>
       <c r="C3" s="3">
-        <v>43908.0</v>
+        <v>43908</v>
       </c>
       <c r="D3" s="1">
-        <v>2500.0</v>
+        <v>2500</v>
       </c>
       <c r="E3" s="4">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="7">
@@ -414,26 +411,26 @@
         <v>6643</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
+        <f t="shared" si="0"/>
+        <v>6643</v>
+      </c>
+      <c r="B4" s="8">
         <f t="shared" si="1"/>
-        <v>6643</v>
-      </c>
-      <c r="B4" s="9">
-        <f t="shared" si="2"/>
         <v>43908</v>
       </c>
       <c r="C4" s="3">
-        <v>44087.0</v>
+        <v>44087</v>
       </c>
       <c r="D4" s="1">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="4">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="7">
@@ -441,26 +438,26 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
+        <f t="shared" si="0"/>
+        <v>1874</v>
+      </c>
+      <c r="B5" s="8">
         <f t="shared" si="1"/>
-        <v>1874</v>
-      </c>
-      <c r="B5" s="9">
-        <f t="shared" si="2"/>
         <v>44087</v>
       </c>
       <c r="C5" s="3">
-        <v>44152.0</v>
+        <v>44152</v>
       </c>
       <c r="D5" s="1">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="E5" s="4">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="7">
@@ -468,252 +465,244 @@
         <v>397</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>10000.0</v>
+        <v>10000</v>
       </c>
       <c r="B9" s="3">
-        <v>43831.0</v>
+        <v>43831</v>
       </c>
       <c r="C9" s="3">
-        <v>43876.0</v>
+        <v>43876</v>
       </c>
       <c r="D9" s="1">
-        <v>1000.0</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.008</v>
+        <v>1000</v>
+      </c>
+      <c r="E9" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7">
         <f>A9-D9+120</f>
         <v>9120</v>
       </c>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" ref="A10:A12" si="3">H9</f>
+        <f t="shared" ref="A10:A12" si="2">H9</f>
         <v>9120</v>
       </c>
-      <c r="B10" s="9">
-        <f t="shared" ref="B10:B12" si="4">C9</f>
+      <c r="B10" s="8">
+        <f t="shared" ref="B10:B12" si="3">C9</f>
         <v>43876</v>
       </c>
       <c r="C10" s="3">
-        <v>43908.0</v>
+        <v>43908</v>
       </c>
       <c r="D10" s="1">
-        <v>2500.0</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.008</v>
+        <v>2500</v>
+      </c>
+      <c r="E10" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="7">
         <f>A10-D10+77</f>
         <v>6697</v>
       </c>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
+        <f t="shared" si="2"/>
+        <v>6697</v>
+      </c>
+      <c r="B11" s="8">
         <f t="shared" si="3"/>
-        <v>6697</v>
-      </c>
-      <c r="B11" s="9">
-        <f t="shared" si="4"/>
         <v>43908</v>
       </c>
       <c r="C11" s="3">
-        <v>44087.0</v>
+        <v>44087</v>
       </c>
       <c r="D11" s="1">
-        <v>5000.0</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0.008</v>
+        <v>5000</v>
+      </c>
+      <c r="E11" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="7">
         <f>A11-D11+319</f>
         <v>2016</v>
       </c>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
+        <f t="shared" si="2"/>
+        <v>2016</v>
+      </c>
+      <c r="B12" s="8">
         <f t="shared" si="3"/>
-        <v>2016</v>
-      </c>
-      <c r="B12" s="9">
-        <f t="shared" si="4"/>
         <v>44087</v>
       </c>
       <c r="C12" s="3">
-        <v>44152.0</v>
+        <v>44152</v>
       </c>
       <c r="D12" s="1">
-        <v>1500.0</v>
-      </c>
-      <c r="E12" s="11">
-        <v>0.008</v>
+        <v>1500</v>
+      </c>
+      <c r="E12" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="7">
         <f>A12-D12+39</f>
         <v>555</v>
       </c>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>10000.0</v>
+        <v>10000</v>
       </c>
       <c r="B15" s="3">
-        <v>43831.0</v>
+        <v>43831</v>
       </c>
       <c r="C15" s="3">
-        <v>43876.0</v>
+        <v>43876</v>
       </c>
       <c r="D15" s="1">
-        <v>1000.0</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0.008</v>
+        <v>1000</v>
+      </c>
+      <c r="E15" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="7">
         <f>A15-D15+40</f>
         <v>9040</v>
       </c>
-      <c r="N15" s="8"/>
-    </row>
-    <row r="16">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" ref="A16:A18" si="5">H15</f>
+        <f t="shared" ref="A16:A18" si="4">H15</f>
         <v>9040</v>
       </c>
-      <c r="B16" s="9">
-        <f t="shared" ref="B16:B18" si="6">C15</f>
+      <c r="B16" s="8">
+        <f t="shared" ref="B16:B18" si="5">C15</f>
         <v>43876</v>
       </c>
       <c r="C16" s="3">
-        <v>43908.0</v>
+        <v>43908</v>
       </c>
       <c r="D16" s="1">
-        <v>2500.0</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.008</v>
+        <v>2500</v>
+      </c>
+      <c r="E16" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="7">
         <f>A16-D16+25</f>
         <v>6565</v>
       </c>
-      <c r="N16" s="8"/>
-    </row>
-    <row r="17">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
+        <f t="shared" si="4"/>
+        <v>6565</v>
+      </c>
+      <c r="B17" s="8">
         <f t="shared" si="5"/>
-        <v>6565</v>
-      </c>
-      <c r="B17" s="9">
-        <f t="shared" si="6"/>
         <v>43908</v>
       </c>
       <c r="C17" s="3">
-        <v>44087.0</v>
+        <v>44087</v>
       </c>
       <c r="D17" s="1">
-        <v>5000.0</v>
-      </c>
-      <c r="E17" s="11">
-        <v>0.008</v>
+        <v>5000</v>
+      </c>
+      <c r="E17" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="7">
         <f>A17-D17+104</f>
         <v>1669</v>
       </c>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
+        <f t="shared" si="4"/>
+        <v>1669</v>
+      </c>
+      <c r="B18" s="8">
         <f t="shared" si="5"/>
-        <v>1669</v>
-      </c>
-      <c r="B18" s="9">
-        <f t="shared" si="6"/>
         <v>44087</v>
       </c>
       <c r="C18" s="3">
-        <v>44152.0</v>
+        <v>44152</v>
       </c>
       <c r="D18" s="1">
-        <v>1500.0</v>
-      </c>
-      <c r="E18" s="11">
-        <v>0.008</v>
+        <v>1500</v>
+      </c>
+      <c r="E18" s="10">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="7">
         <f>A18-D18+9</f>
         <v>178</v>
       </c>
-      <c r="N18" s="8"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>